<commit_message>
version with 2 ref files
</commit_message>
<xml_diff>
--- a/target.xlsx
+++ b/target.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nikolamotor-my.sharepoint.com/personal/pierre_congiu_nikolamotor_com/Documents/Documents/Repositories/excel_column_cleaner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\excel-backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A5886DB2-F11B-4167-BEF9-73C9AF810C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F66EEE94-4287-4267-90D4-09D07F15C8C1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE88A7CC-6B8E-433A-BD7E-4D18BFFDEC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Index:</t>
   </si>
@@ -78,13 +78,16 @@
     <t>8 boulevard Qorvo</t>
   </si>
   <si>
-    <t>Inandout</t>
-  </si>
-  <si>
     <t>address to change</t>
   </si>
   <si>
     <t>Burger King greensboro to change</t>
+  </si>
+  <si>
+    <t>sdcasdc</t>
+  </si>
+  <si>
+    <t>sdcasddd</t>
   </si>
 </sst>
 </file>
@@ -410,20 +413,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,29 +440,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>25962</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -469,8 +476,11 @@
       <c r="D4">
         <v>67978</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -483,8 +493,11 @@
       <c r="D5">
         <v>87631</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -494,8 +507,11 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -508,8 +524,11 @@
       <c r="D7">
         <v>84201</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -522,8 +541,11 @@
       <c r="D8">
         <v>84938</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -533,16 +555,22 @@
       <c r="D9">
         <v>80357</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -554,6 +582,19 @@
       </c>
       <c r="D11">
         <v>14366</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>